<commit_message>
Update TechnoterBurnDownChart 3 Juni 2014
</commit_message>
<xml_diff>
--- a/technoterburndownchart.xlsx
+++ b/technoterburndownchart.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\[CAMPUS]\[BAHANKULIAH]\[IV]\[TKPPL][AXA]\technoter\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\[CAMPUS]\[BAHANKULIAH]\[IV]\[TKPPL][AXA]\[TUGASBESAR]\technoter\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -41,15 +41,6 @@
     <t>Pengumpulan Requirements</t>
   </si>
   <si>
-    <t>Pengumpulan user requirements</t>
-  </si>
-  <si>
-    <t>Pengumpulan system requirements</t>
-  </si>
-  <si>
-    <t>Pengumpulan functional requirements</t>
-  </si>
-  <si>
     <t>Pembuatan Design</t>
   </si>
   <si>
@@ -102,6 +93,15 @@
   </si>
   <si>
     <t>Prediction</t>
+  </si>
+  <si>
+    <t>Pengumpulan user requirements dan pembuatan slide</t>
+  </si>
+  <si>
+    <t>Pengumpulan system requirements dan pembuatan slide</t>
+  </si>
+  <si>
+    <t>Pengumpulan functional requirements dan pembuatan slide</t>
   </si>
 </sst>
 </file>
@@ -613,7 +613,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>3</c:v>
@@ -632,11 +632,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="287722808"/>
-        <c:axId val="287723984"/>
+        <c:axId val="256320152"/>
+        <c:axId val="256320544"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="287722808"/>
+        <c:axId val="256320152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -678,7 +678,7 @@
             <a:endParaRPr lang="id-ID"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="287723984"/>
+        <c:crossAx val="256320544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -686,7 +686,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="287723984"/>
+        <c:axId val="256320544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -736,7 +736,7 @@
             <a:endParaRPr lang="id-ID"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="287722808"/>
+        <c:crossAx val="256320152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1668,14 +1668,14 @@
   <dimension ref="A1:P71"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection sqref="A1:N1"/>
+      <selection activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32.42578125" style="3" customWidth="1"/>
     <col min="2" max="2" width="26.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="41" style="3" customWidth="1"/>
+    <col min="3" max="3" width="59.140625" style="3" customWidth="1"/>
     <col min="4" max="4" width="14.7109375" style="1" customWidth="1"/>
     <col min="5" max="14" width="13.5703125" style="1" customWidth="1"/>
     <col min="15" max="16" width="13.5703125" style="3" customWidth="1"/>
@@ -1713,7 +1713,7 @@
         <v>2</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E4" s="8">
         <v>41804</v>
@@ -1754,13 +1754,13 @@
     </row>
     <row r="5" spans="1:16" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="D5" s="2">
         <v>6</v>
@@ -1775,7 +1775,9 @@
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
-      <c r="O5" s="2"/>
+      <c r="O5" s="2">
+        <v>2</v>
+      </c>
       <c r="P5" s="2">
         <v>1</v>
       </c>
@@ -1784,7 +1786,7 @@
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="D6" s="2">
         <v>6</v>
@@ -1799,7 +1801,9 @@
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
-      <c r="O6" s="2"/>
+      <c r="O6" s="2">
+        <v>2</v>
+      </c>
       <c r="P6" s="2">
         <v>1</v>
       </c>
@@ -1808,7 +1812,7 @@
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="D7" s="2">
         <v>6</v>
@@ -1823,7 +1827,9 @@
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
-      <c r="O7" s="2"/>
+      <c r="O7" s="2">
+        <v>2</v>
+      </c>
       <c r="P7" s="2">
         <v>1</v>
       </c>
@@ -1850,13 +1856,13 @@
     </row>
     <row r="9" spans="1:16" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B9" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>8</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>11</v>
       </c>
       <c r="D9" s="2">
         <v>8</v>
@@ -1880,7 +1886,7 @@
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D10" s="2">
         <v>12</v>
@@ -1904,7 +1910,7 @@
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D11" s="2">
         <v>8</v>
@@ -1944,13 +1950,13 @@
     </row>
     <row r="13" spans="1:16" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D13" s="2">
         <v>6</v>
@@ -1974,7 +1980,7 @@
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D14" s="2">
         <v>8</v>
@@ -1998,7 +2004,7 @@
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D15" s="2">
         <v>6</v>
@@ -2038,13 +2044,13 @@
     </row>
     <row r="17" spans="1:16" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D17" s="2">
         <v>2</v>
@@ -2068,7 +2074,7 @@
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D18" s="2">
         <v>1</v>
@@ -2110,7 +2116,7 @@
     </row>
     <row r="20" spans="1:16" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B20" s="10"/>
       <c r="C20" s="10"/>
@@ -2169,7 +2175,7 @@
     </row>
     <row r="21" spans="1:16" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B21" s="10"/>
       <c r="C21" s="10"/>
@@ -2219,7 +2225,7 @@
       </c>
       <c r="O21" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="P21" s="2">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
Update TechnoterBurnDownChart 4 Juni 2014
</commit_message>
<xml_diff>
--- a/technoterburndownchart.xlsx
+++ b/technoterburndownchart.xlsx
@@ -610,7 +610,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>6</c:v>
@@ -632,11 +632,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="256320152"/>
-        <c:axId val="256320544"/>
+        <c:axId val="255052448"/>
+        <c:axId val="255057544"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="256320152"/>
+        <c:axId val="255052448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -678,7 +678,7 @@
             <a:endParaRPr lang="id-ID"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="256320544"/>
+        <c:crossAx val="255057544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -686,7 +686,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="256320544"/>
+        <c:axId val="255057544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -736,7 +736,7 @@
             <a:endParaRPr lang="id-ID"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="256320152"/>
+        <c:crossAx val="255052448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1667,8 +1667,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O21" sqref="O21"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -1774,7 +1774,9 @@
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
+      <c r="N5" s="2">
+        <v>3</v>
+      </c>
       <c r="O5" s="2">
         <v>2</v>
       </c>
@@ -1800,7 +1802,9 @@
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
+      <c r="N6" s="2">
+        <v>3</v>
+      </c>
       <c r="O6" s="2">
         <v>2</v>
       </c>
@@ -1826,7 +1830,9 @@
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
+      <c r="N7" s="2">
+        <v>3</v>
+      </c>
       <c r="O7" s="2">
         <v>2</v>
       </c>
@@ -1876,8 +1882,12 @@
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
-      <c r="O9" s="2"/>
+      <c r="N9" s="2">
+        <v>0</v>
+      </c>
+      <c r="O9" s="2">
+        <v>0</v>
+      </c>
       <c r="P9" s="2">
         <v>0</v>
       </c>
@@ -1900,8 +1910,12 @@
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
-      <c r="O10" s="2"/>
+      <c r="N10" s="2">
+        <v>0</v>
+      </c>
+      <c r="O10" s="2">
+        <v>0</v>
+      </c>
       <c r="P10" s="2">
         <v>0</v>
       </c>
@@ -1924,8 +1938,12 @@
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
-      <c r="O11" s="2"/>
+      <c r="N11" s="2">
+        <v>0</v>
+      </c>
+      <c r="O11" s="2">
+        <v>0</v>
+      </c>
       <c r="P11" s="2">
         <v>0</v>
       </c>
@@ -1970,8 +1988,12 @@
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
-      <c r="N13" s="2"/>
-      <c r="O13" s="2"/>
+      <c r="N13" s="2">
+        <v>2</v>
+      </c>
+      <c r="O13" s="2">
+        <v>0</v>
+      </c>
       <c r="P13" s="2">
         <v>0</v>
       </c>
@@ -1994,8 +2016,12 @@
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
-      <c r="N14" s="2"/>
-      <c r="O14" s="2"/>
+      <c r="N14" s="2">
+        <v>0</v>
+      </c>
+      <c r="O14" s="2">
+        <v>0</v>
+      </c>
       <c r="P14" s="2">
         <v>0</v>
       </c>
@@ -2018,8 +2044,12 @@
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
-      <c r="N15" s="2"/>
-      <c r="O15" s="2"/>
+      <c r="N15" s="2">
+        <v>0</v>
+      </c>
+      <c r="O15" s="2">
+        <v>0</v>
+      </c>
       <c r="P15" s="2">
         <v>0</v>
       </c>
@@ -2064,8 +2094,12 @@
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
-      <c r="N17" s="2"/>
-      <c r="O17" s="2"/>
+      <c r="N17" s="2">
+        <v>0</v>
+      </c>
+      <c r="O17" s="2">
+        <v>0</v>
+      </c>
       <c r="P17" s="2">
         <v>0</v>
       </c>
@@ -2088,8 +2122,12 @@
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
       <c r="M18" s="2"/>
-      <c r="N18" s="2"/>
-      <c r="O18" s="2"/>
+      <c r="N18" s="2">
+        <v>0</v>
+      </c>
+      <c r="O18" s="2">
+        <v>0</v>
+      </c>
       <c r="P18" s="2">
         <v>0</v>
       </c>
@@ -2221,7 +2259,7 @@
       </c>
       <c r="N21" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="O21" s="2">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
Perbaikan TechnoterBurnDownChart 5 Juni 2014
</commit_message>
<xml_diff>
--- a/technoterburndownchart.xlsx
+++ b/technoterburndownchart.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johan\technoter_TKPPL-utama-\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\[CAMPUS]\[BAHANKULIAH]\[IV]\[TKPPL][AXA]\[TUGASBESAR]\technoter\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -583,34 +583,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>11</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>6</c:v>
@@ -632,11 +632,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="271527920"/>
-        <c:axId val="271525176"/>
+        <c:axId val="263568200"/>
+        <c:axId val="263572120"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="271527920"/>
+        <c:axId val="263568200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -678,7 +678,7 @@
             <a:endParaRPr lang="id-ID"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="271525176"/>
+        <c:crossAx val="263572120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -686,7 +686,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="271525176"/>
+        <c:axId val="263572120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -736,7 +736,7 @@
             <a:endParaRPr lang="id-ID"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="271527920"/>
+        <c:crossAx val="263568200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1667,8 +1667,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P71"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="S9" sqref="S9"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P34" sqref="P34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -1773,12 +1773,14 @@
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
+      <c r="M5" s="2">
+        <v>0</v>
+      </c>
       <c r="N5" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O5" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P5" s="2">
         <v>1</v>
@@ -1801,12 +1803,14 @@
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
+      <c r="M6" s="2">
+        <v>0</v>
+      </c>
       <c r="N6" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O6" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P6" s="2">
         <v>1</v>
@@ -1829,12 +1833,14 @@
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
+      <c r="M7" s="2">
+        <v>0</v>
+      </c>
       <c r="N7" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O7" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P7" s="2">
         <v>1</v>
@@ -1942,7 +1948,7 @@
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
       <c r="M11" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N11" s="2">
         <v>0</v>
@@ -1993,9 +1999,11 @@
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
-      <c r="M13" s="2"/>
+      <c r="M13" s="2">
+        <v>0</v>
+      </c>
       <c r="N13" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O13" s="2">
         <v>0</v>
@@ -2021,7 +2029,9 @@
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
-      <c r="M14" s="2"/>
+      <c r="M14" s="2">
+        <v>0</v>
+      </c>
       <c r="N14" s="2">
         <v>0</v>
       </c>
@@ -2049,7 +2059,9 @@
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
-      <c r="M15" s="2"/>
+      <c r="M15" s="2">
+        <v>0</v>
+      </c>
       <c r="N15" s="2">
         <v>0</v>
       </c>
@@ -2099,7 +2111,9 @@
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
-      <c r="M17" s="2"/>
+      <c r="M17" s="2">
+        <v>0</v>
+      </c>
       <c r="N17" s="2">
         <v>0</v>
       </c>
@@ -2127,7 +2141,9 @@
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
-      <c r="M18" s="2"/>
+      <c r="M18" s="2">
+        <v>0</v>
+      </c>
       <c r="N18" s="2">
         <v>0</v>
       </c>
@@ -2228,51 +2244,51 @@
         <v>69</v>
       </c>
       <c r="E21" s="2">
-        <f>(SUM(E17:E18)+SUM(E13:E15)+SUM(E9:E11)+SUM(E5:E7))</f>
-        <v>0</v>
+        <f t="shared" ref="E21:N21" si="1">(SUM(E17:E18)+SUM(E13:E15)+SUM(E9:E11)+SUM(E5:E7))+F21</f>
+        <v>19</v>
       </c>
       <c r="F21" s="2">
-        <f t="shared" ref="F21:P21" si="1">(SUM(F17:F18)+SUM(F13:F15)+SUM(F9:F11)+SUM(F5:F7))</f>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>19</v>
       </c>
       <c r="G21" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="H21" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="I21" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="J21" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="K21" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="L21" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="M21" s="2">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="N21" s="2">
         <f t="shared" si="1"/>
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="O21" s="2">
-        <f t="shared" si="1"/>
+        <f>(SUM(O17:O18)+SUM(O13:O15)+SUM(O9:O11)+SUM(O5:O7))+P21</f>
         <v>6</v>
       </c>
       <c r="P21" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="F21:P21" si="2">(SUM(P17:P18)+SUM(P13:P15)+SUM(P9:P11)+SUM(P5:P7))</f>
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
input data burndown chart
</commit_message>
<xml_diff>
--- a/technoterburndownchart.xlsx
+++ b/technoterburndownchart.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PramaDaeli\Documents\GitHub\technoter_PramaDaeli\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sepna Angel U . S\Documents\GitHub\UTAMA\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -583,13 +583,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>48</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>48</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>48</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>48</c:v>
@@ -632,11 +632,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="275360984"/>
-        <c:axId val="276496360"/>
+        <c:axId val="313877960"/>
+        <c:axId val="313873256"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="275360984"/>
+        <c:axId val="313877960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -678,7 +678,7 @@
             <a:endParaRPr lang="id-ID"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="276496360"/>
+        <c:crossAx val="313873256"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -686,7 +686,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="276496360"/>
+        <c:axId val="313873256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -736,7 +736,7 @@
             <a:endParaRPr lang="id-ID"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="275360984"/>
+        <c:crossAx val="313877960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1667,8 +1667,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P71"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -1768,7 +1768,9 @@
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
+      <c r="H5" s="2">
+        <v>0</v>
+      </c>
       <c r="I5" s="2">
         <v>0</v>
       </c>
@@ -1806,7 +1808,9 @@
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
+      <c r="H6" s="2">
+        <v>0</v>
+      </c>
       <c r="I6" s="2">
         <v>0</v>
       </c>
@@ -1844,7 +1848,9 @@
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
+      <c r="H7" s="2">
+        <v>0</v>
+      </c>
       <c r="I7" s="2">
         <v>0</v>
       </c>
@@ -1906,7 +1912,9 @@
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
+      <c r="H9" s="2">
+        <v>0</v>
+      </c>
       <c r="I9" s="2">
         <v>0</v>
       </c>
@@ -1944,7 +1952,9 @@
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
+      <c r="H10" s="2">
+        <v>0</v>
+      </c>
       <c r="I10" s="2">
         <v>0</v>
       </c>
@@ -1982,7 +1992,9 @@
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
+      <c r="H11" s="2">
+        <v>0</v>
+      </c>
       <c r="I11" s="2">
         <v>0</v>
       </c>
@@ -2183,8 +2195,12 @@
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
+      <c r="G17" s="2">
+        <v>2</v>
+      </c>
+      <c r="H17" s="2">
+        <v>0</v>
+      </c>
       <c r="I17" s="2">
         <v>0</v>
       </c>
@@ -2221,8 +2237,12 @@
       </c>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
+      <c r="G18" s="2">
+        <v>3</v>
+      </c>
+      <c r="H18" s="2">
+        <v>0</v>
+      </c>
       <c r="I18" s="2">
         <v>0</v>
       </c>
@@ -2339,15 +2359,15 @@
       </c>
       <c r="E21" s="2">
         <f t="shared" ref="E21:N21" si="1">(SUM(E17:E18)+SUM(E13:E15)+SUM(E9:E11)+SUM(E5:E7))+F21</f>
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="F21" s="2">
         <f t="shared" si="1"/>
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="G21" s="2">
         <f t="shared" si="1"/>
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="H21" s="2">
         <f t="shared" si="1"/>

</xml_diff>